<commit_message>
Cleanup & Allen Stims
</commit_message>
<xml_diff>
--- a/IETwo/analysis/GroupBehavior.xlsx
+++ b/IETwo/analysis/GroupBehavior.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achen52\Documents\GitHub\movingstims\IETwo\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhshaw\Documents\GitHub\movingstims\IETwo\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -408,12 +408,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -432,12 +432,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -456,12 +456,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -503,7 +503,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -598,7 +598,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C988-4FE1-88C3-A0B9DCE61C5E}"/>
             </c:ext>
@@ -636,12 +636,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -660,12 +660,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -684,12 +684,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -731,7 +731,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -826,7 +826,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C988-4FE1-88C3-A0B9DCE61C5E}"/>
             </c:ext>
@@ -864,12 +864,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -888,12 +888,12 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-C988-4FE1-88C3-A0B9DCE61C5E}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-C988-4FE1-88C3-A0B9DCE61C5E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -935,7 +935,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="0"/>
@@ -1031,7 +1031,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C988-4FE1-88C3-A0B9DCE61C5E}"/>
             </c:ext>
@@ -1048,11 +1048,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="492701320"/>
-        <c:axId val="492698696"/>
+        <c:axId val="97467760"/>
+        <c:axId val="172660224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="492701320"/>
+        <c:axId val="97467760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492698696"/>
+        <c:crossAx val="172660224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1170,7 +1170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492698696"/>
+        <c:axId val="172660224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1268,7 +1268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492701320"/>
+        <c:crossAx val="97467760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1356,7 +1356,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1489,7 +1489,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8FC5-4B71-A175-6365D29783F4}"/>
             </c:ext>
@@ -1558,7 +1558,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-8FC5-4B71-A175-6365D29783F4}"/>
             </c:ext>
@@ -1627,7 +1627,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-8FC5-4B71-A175-6365D29783F4}"/>
             </c:ext>
@@ -1643,11 +1643,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="494146488"/>
-        <c:axId val="494148456"/>
+        <c:axId val="171545192"/>
+        <c:axId val="171545584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494146488"/>
+        <c:axId val="171545192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,7 +1734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494148456"/>
+        <c:crossAx val="171545584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1742,7 +1742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="494148456"/>
+        <c:axId val="171545584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-0.1"/>
@@ -1843,7 +1843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494146488"/>
+        <c:crossAx val="171545192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1926,7 +1926,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2065,7 +2065,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5ACB-438C-9A70-88B187D3C341}"/>
             </c:ext>
@@ -2134,7 +2134,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5ACB-438C-9A70-88B187D3C341}"/>
             </c:ext>
@@ -2221,7 +2221,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5ACB-438C-9A70-88B187D3C341}"/>
             </c:ext>
@@ -2237,11 +2237,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="495890168"/>
-        <c:axId val="495891480"/>
+        <c:axId val="206907664"/>
+        <c:axId val="206908056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="495890168"/>
+        <c:axId val="206907664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,7 +2337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495891480"/>
+        <c:crossAx val="206908056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2345,7 +2345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="495891480"/>
+        <c:axId val="206908056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -2448,7 +2448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495890168"/>
+        <c:crossAx val="206907664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2530,7 +2530,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2666,7 +2666,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EF25-4D3C-B7A3-1D61933E2084}"/>
             </c:ext>
@@ -2682,11 +2682,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="500295648"/>
-        <c:axId val="500294664"/>
+        <c:axId val="206908840"/>
+        <c:axId val="206909232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="500295648"/>
+        <c:axId val="206908840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,7 +2728,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500294664"/>
+        <c:crossAx val="206909232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2736,7 +2736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="500294664"/>
+        <c:axId val="206909232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2787,7 +2787,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500295648"/>
+        <c:crossAx val="206908840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>